<commit_message>
Changing way of downloading data
</commit_message>
<xml_diff>
--- a/gus.xlsx
+++ b/gus.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Location</t>
   </si>
@@ -22,12 +22,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Unit Measure</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>Liczba lokali mieszkalnych sprzedanych w ramach transakcji rynkowych (szt.)</t>
   </si>
   <si>
@@ -58,6 +52,24 @@
     <t>Przeciętna powierzchnia użytkowa 1 mieszkania oddanego do użytkowania (m2)</t>
   </si>
   <si>
+    <t>Przeciętna liczba izb w 1 mieszkaniu oddanym do użytkowania</t>
+  </si>
+  <si>
+    <t>Nowe budynki mieszkalne na 1000 ludności</t>
+  </si>
+  <si>
+    <t>Udział mieszkań oddanych do użytkowania w nowych budynkach jednorodzinnych w łącznej liczbie mieszkań oddanych do użytkowania w nowych budynkach mieszkalnych (%)</t>
+  </si>
+  <si>
+    <t>Udział mieszkań oddanych do użytkowania w nowych budynkach wielorodzinnych w łącznej liczbie mieszkań oddanych do użytkowania w nowych budynkach mieszkalnych (%)</t>
+  </si>
+  <si>
+    <t>Przeciętny czas trwania budowy nowych budynków mieszkalnych jednorodzinnych (mc)</t>
+  </si>
+  <si>
+    <t>Grunty pozostające w zasobie gmin pod budownictwo mieszkaniowe (ha)</t>
+  </si>
+  <si>
     <t>MAŁOPOLSKIE</t>
   </si>
   <si>
@@ -107,54 +119,6 @@
   </si>
   <si>
     <t>2020</t>
-  </si>
-  <si>
-    <t>2020MAŁOPOLSKIE</t>
-  </si>
-  <si>
-    <t>2020ŚLĄSKIE</t>
-  </si>
-  <si>
-    <t>2020LUBUSKIE</t>
-  </si>
-  <si>
-    <t>2020WIELKOPOLSKIE</t>
-  </si>
-  <si>
-    <t>2020ZACHODNIOPOMORSKIE</t>
-  </si>
-  <si>
-    <t>2020DOLNOŚLĄSKIE</t>
-  </si>
-  <si>
-    <t>2020OPOLSKIE</t>
-  </si>
-  <si>
-    <t>2020KUJAWSKO-POMORSKIE</t>
-  </si>
-  <si>
-    <t>2020POMORSKIE</t>
-  </si>
-  <si>
-    <t>2020WARMIŃSKO-MAZURSKIE</t>
-  </si>
-  <si>
-    <t>2020ŁÓDZKIE</t>
-  </si>
-  <si>
-    <t>2020ŚWIĘTOKRZYSKIE</t>
-  </si>
-  <si>
-    <t>2020LUBELSKIE</t>
-  </si>
-  <si>
-    <t>2020PODKARPACKIE</t>
-  </si>
-  <si>
-    <t>2020PODLASKIE</t>
-  </si>
-  <si>
-    <t>2020MAZOWIECKIE</t>
   </si>
 </sst>
 </file>
@@ -512,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,709 +525,961 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>16549</v>
+      </c>
+      <c r="E2">
+        <v>876127.9</v>
       </c>
       <c r="F2">
-        <v>16549</v>
+        <v>383846</v>
       </c>
       <c r="G2">
-        <v>876127.9</v>
+        <v>7296</v>
       </c>
       <c r="H2">
-        <v>383846</v>
+        <v>7250</v>
       </c>
       <c r="I2">
-        <v>7296</v>
+        <v>5.8</v>
       </c>
       <c r="J2">
-        <v>7250</v>
+        <v>57.7</v>
       </c>
       <c r="K2">
-        <v>5.8</v>
+        <v>1372</v>
       </c>
       <c r="L2">
-        <v>57.7</v>
+        <v>533</v>
       </c>
       <c r="M2">
-        <v>1372</v>
+        <v>92.3</v>
       </c>
       <c r="N2">
-        <v>533</v>
+        <v>3.9</v>
       </c>
       <c r="O2">
-        <v>92.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>2.5</v>
+      </c>
+      <c r="P2">
+        <v>0.5</v>
+      </c>
+      <c r="Q2">
+        <v>0.5</v>
+      </c>
+      <c r="R2">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="S2">
+        <v>3603.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>17541</v>
+      </c>
+      <c r="E3">
+        <v>917179.2</v>
       </c>
       <c r="F3">
-        <v>17541</v>
+        <v>208519</v>
       </c>
       <c r="G3">
-        <v>917179.2</v>
+        <v>3960</v>
       </c>
       <c r="H3">
-        <v>208519</v>
+        <v>3988</v>
       </c>
       <c r="I3">
-        <v>3960</v>
+        <v>4.1</v>
       </c>
       <c r="J3">
-        <v>3988</v>
+        <v>41.3</v>
       </c>
       <c r="K3">
-        <v>4.1</v>
+        <v>1106</v>
       </c>
       <c r="L3">
-        <v>41.3</v>
+        <v>395.8</v>
       </c>
       <c r="M3">
-        <v>1106</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="N3">
-        <v>395.8</v>
+        <v>4</v>
       </c>
       <c r="O3">
-        <v>95.90000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>2.1</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3">
+        <v>0.5</v>
+      </c>
+      <c r="R3">
+        <v>44.7</v>
+      </c>
+      <c r="S3">
+        <v>3387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>6319</v>
+      </c>
+      <c r="E4">
+        <v>333262.7</v>
       </c>
       <c r="F4">
-        <v>6319</v>
+        <v>200453</v>
       </c>
       <c r="G4">
-        <v>333262.7</v>
+        <v>3909</v>
       </c>
       <c r="H4">
-        <v>200453</v>
+        <v>3801</v>
       </c>
       <c r="I4">
-        <v>3909</v>
+        <v>5.2</v>
       </c>
       <c r="J4">
-        <v>3801</v>
+        <v>51.8</v>
       </c>
       <c r="K4">
-        <v>5.2</v>
+        <v>1470</v>
       </c>
       <c r="L4">
-        <v>51.8</v>
+        <v>445.6</v>
       </c>
       <c r="M4">
-        <v>1470</v>
+        <v>86</v>
       </c>
       <c r="N4">
-        <v>445.6</v>
+        <v>3.9</v>
       </c>
       <c r="O4">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>2.5</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>0.5</v>
+      </c>
+      <c r="R4">
+        <v>43</v>
+      </c>
+      <c r="S4">
+        <v>1743.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>16508</v>
+      </c>
+      <c r="E5">
+        <v>957678.2</v>
       </c>
       <c r="F5">
-        <v>16508</v>
+        <v>276151</v>
       </c>
       <c r="G5">
-        <v>957678.2</v>
+        <v>4626</v>
       </c>
       <c r="H5">
-        <v>276151</v>
+        <v>4760</v>
       </c>
       <c r="I5">
-        <v>4626</v>
+        <v>6.3</v>
       </c>
       <c r="J5">
-        <v>4760</v>
+        <v>62.7</v>
       </c>
       <c r="K5">
-        <v>6.3</v>
+        <v>1572</v>
       </c>
       <c r="L5">
-        <v>62.7</v>
+        <v>575</v>
       </c>
       <c r="M5">
-        <v>1572</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="N5">
-        <v>575</v>
+        <v>3.9</v>
       </c>
       <c r="O5">
-        <v>91.59999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>3.1</v>
+      </c>
+      <c r="P5">
+        <v>0.6</v>
+      </c>
+      <c r="Q5">
+        <v>0.4</v>
+      </c>
+      <c r="R5">
+        <v>32.8</v>
+      </c>
+      <c r="S5">
+        <v>1343.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>6492</v>
+      </c>
+      <c r="E6">
+        <v>348804.8</v>
       </c>
       <c r="F6">
-        <v>6492</v>
+        <v>256657</v>
       </c>
       <c r="G6">
-        <v>348804.8</v>
+        <v>4224</v>
       </c>
       <c r="H6">
-        <v>256657</v>
+        <v>4777</v>
       </c>
       <c r="I6">
-        <v>4224</v>
+        <v>5.4</v>
       </c>
       <c r="J6">
-        <v>4777</v>
+        <v>54</v>
       </c>
       <c r="K6">
-        <v>5.4</v>
+        <v>1463</v>
       </c>
       <c r="L6">
-        <v>54</v>
+        <v>420.3</v>
       </c>
       <c r="M6">
-        <v>1463</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="N6">
-        <v>420.3</v>
+        <v>3.4</v>
       </c>
       <c r="O6">
-        <v>77.90000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>1.8</v>
+      </c>
+      <c r="P6">
+        <v>0.4</v>
+      </c>
+      <c r="Q6">
+        <v>0.6</v>
+      </c>
+      <c r="R6">
+        <v>35.1</v>
+      </c>
+      <c r="S6">
+        <v>2344.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>20386</v>
+      </c>
+      <c r="E7">
+        <v>1133930.8</v>
       </c>
       <c r="F7">
-        <v>20386</v>
+        <v>268487</v>
       </c>
       <c r="G7">
-        <v>1133930.8</v>
+        <v>4720</v>
       </c>
       <c r="H7">
-        <v>268487</v>
+        <v>4827</v>
       </c>
       <c r="I7">
-        <v>4720</v>
+        <v>7.5</v>
       </c>
       <c r="J7">
-        <v>4827</v>
+        <v>75</v>
       </c>
       <c r="K7">
-        <v>7.5</v>
+        <v>2021</v>
       </c>
       <c r="L7">
-        <v>75</v>
+        <v>609.7</v>
       </c>
       <c r="M7">
-        <v>2021</v>
+        <v>81.3</v>
       </c>
       <c r="N7">
-        <v>609.7</v>
+        <v>3.5</v>
       </c>
       <c r="O7">
-        <v>81.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>2.7</v>
+      </c>
+      <c r="P7">
+        <v>0.4</v>
+      </c>
+      <c r="Q7">
+        <v>0.6</v>
+      </c>
+      <c r="R7">
+        <v>34.4</v>
+      </c>
+      <c r="S7">
+        <v>3270.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>4277</v>
+      </c>
+      <c r="E8">
+        <v>235722.5</v>
       </c>
       <c r="F8">
-        <v>4277</v>
+        <v>210993</v>
       </c>
       <c r="G8">
-        <v>235722.5</v>
+        <v>3922</v>
       </c>
       <c r="H8">
-        <v>210993</v>
+        <v>3828</v>
       </c>
       <c r="I8">
-        <v>3922</v>
+        <v>2.7</v>
       </c>
       <c r="J8">
-        <v>3828</v>
+        <v>27.3</v>
       </c>
       <c r="K8">
-        <v>2.7</v>
+        <v>787</v>
       </c>
       <c r="L8">
-        <v>27.3</v>
+        <v>313.9</v>
       </c>
       <c r="M8">
-        <v>787</v>
+        <v>115.2</v>
       </c>
       <c r="N8">
-        <v>313.9</v>
+        <v>4.6</v>
       </c>
       <c r="O8">
-        <v>115.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>1.8</v>
+      </c>
+      <c r="P8">
+        <v>0.7</v>
+      </c>
+      <c r="Q8">
+        <v>0.3</v>
+      </c>
+      <c r="R8">
+        <v>48.8</v>
+      </c>
+      <c r="S8">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>8346</v>
+      </c>
+      <c r="E9">
+        <v>430630.2</v>
       </c>
       <c r="F9">
-        <v>8346</v>
+        <v>240574</v>
       </c>
       <c r="G9">
-        <v>430630.2</v>
+        <v>4724</v>
       </c>
       <c r="H9">
-        <v>240574</v>
+        <v>4663</v>
       </c>
       <c r="I9">
-        <v>4724</v>
+        <v>4.8</v>
       </c>
       <c r="J9">
-        <v>4663</v>
+        <v>47.5</v>
       </c>
       <c r="K9">
-        <v>4.8</v>
+        <v>1262</v>
       </c>
       <c r="L9">
-        <v>47.5</v>
+        <v>437.4</v>
       </c>
       <c r="M9">
-        <v>1262</v>
+        <v>92</v>
       </c>
       <c r="N9">
-        <v>437.4</v>
+        <v>4</v>
       </c>
       <c r="O9">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>2.4</v>
+      </c>
+      <c r="P9">
+        <v>0.5</v>
+      </c>
+      <c r="Q9">
+        <v>0.5</v>
+      </c>
+      <c r="R9">
+        <v>35.9</v>
+      </c>
+      <c r="S9">
+        <v>607.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>21900</v>
+      </c>
+      <c r="E10">
+        <v>1213189.7</v>
       </c>
       <c r="F10">
-        <v>21900</v>
+        <v>373985</v>
       </c>
       <c r="G10">
-        <v>1213189.7</v>
+        <v>6343</v>
       </c>
       <c r="H10">
-        <v>373985</v>
+        <v>6751</v>
       </c>
       <c r="I10">
-        <v>6343</v>
+        <v>8.1</v>
       </c>
       <c r="J10">
-        <v>6751</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="K10">
-        <v>8.1</v>
+        <v>2024</v>
       </c>
       <c r="L10">
-        <v>80.90000000000001</v>
+        <v>645.2</v>
       </c>
       <c r="M10">
-        <v>2024</v>
+        <v>79.7</v>
       </c>
       <c r="N10">
-        <v>645.2</v>
+        <v>3.4</v>
       </c>
       <c r="O10">
-        <v>79.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>2.8</v>
+      </c>
+      <c r="P10">
+        <v>0.4</v>
+      </c>
+      <c r="Q10">
+        <v>0.6</v>
+      </c>
+      <c r="R10">
+        <v>43.1</v>
+      </c>
+      <c r="S10">
+        <v>2865.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>8947</v>
+      </c>
+      <c r="E11">
+        <v>475172.1</v>
       </c>
       <c r="F11">
-        <v>8947</v>
+        <v>225310</v>
       </c>
       <c r="G11">
-        <v>475172.1</v>
+        <v>4365</v>
       </c>
       <c r="H11">
-        <v>225310</v>
+        <v>4242</v>
       </c>
       <c r="I11">
-        <v>4365</v>
+        <v>4.6</v>
       </c>
       <c r="J11">
-        <v>4242</v>
+        <v>46.5</v>
       </c>
       <c r="K11">
-        <v>4.6</v>
+        <v>1355</v>
       </c>
       <c r="L11">
-        <v>46.5</v>
+        <v>392.7</v>
       </c>
       <c r="M11">
-        <v>1355</v>
+        <v>84.5</v>
       </c>
       <c r="N11">
-        <v>392.7</v>
+        <v>3.8</v>
       </c>
       <c r="O11">
-        <v>84.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>1.7</v>
+      </c>
+      <c r="P11">
+        <v>0.4</v>
+      </c>
+      <c r="Q11">
+        <v>0.6</v>
+      </c>
+      <c r="R11">
+        <v>47.2</v>
+      </c>
+      <c r="S11">
+        <v>1384.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>11232</v>
+      </c>
+      <c r="E12">
+        <v>562315.9</v>
       </c>
       <c r="F12">
-        <v>11232</v>
+        <v>254199</v>
       </c>
       <c r="G12">
-        <v>562315.9</v>
+        <v>5134</v>
       </c>
       <c r="H12">
-        <v>254199</v>
+        <v>5078</v>
       </c>
       <c r="I12">
-        <v>5134</v>
+        <v>4.6</v>
       </c>
       <c r="J12">
-        <v>5078</v>
+        <v>46.5</v>
       </c>
       <c r="K12">
-        <v>4.6</v>
+        <v>1289</v>
       </c>
       <c r="L12">
-        <v>46.5</v>
+        <v>421.4</v>
       </c>
       <c r="M12">
-        <v>1289</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="N12">
-        <v>421.4</v>
+        <v>3.8</v>
       </c>
       <c r="O12">
-        <v>90.59999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>2.1</v>
+      </c>
+      <c r="P12">
+        <v>0.5</v>
+      </c>
+      <c r="Q12">
+        <v>0.5</v>
+      </c>
+      <c r="R12">
+        <v>47.9</v>
+      </c>
+      <c r="S12">
+        <v>1950.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>3087</v>
+      </c>
+      <c r="E13">
+        <v>162484.7</v>
       </c>
       <c r="F13">
-        <v>3087</v>
+        <v>247876</v>
       </c>
       <c r="G13">
-        <v>162484.7</v>
+        <v>4839</v>
       </c>
       <c r="H13">
-        <v>247876</v>
+        <v>4709</v>
       </c>
       <c r="I13">
-        <v>4839</v>
+        <v>3.3</v>
       </c>
       <c r="J13">
-        <v>4709</v>
+        <v>33</v>
       </c>
       <c r="K13">
-        <v>3.3</v>
+        <v>950</v>
       </c>
       <c r="L13">
-        <v>33</v>
+        <v>333.3</v>
       </c>
       <c r="M13">
-        <v>950</v>
+        <v>101.1</v>
       </c>
       <c r="N13">
-        <v>333.3</v>
+        <v>4.4</v>
       </c>
       <c r="O13">
-        <v>101.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>1.9</v>
+      </c>
+      <c r="P13">
+        <v>0.6</v>
+      </c>
+      <c r="Q13">
+        <v>0.4</v>
+      </c>
+      <c r="R13">
+        <v>70.5</v>
+      </c>
+      <c r="S13">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>7860</v>
+      </c>
+      <c r="E14">
+        <v>408162.2</v>
       </c>
       <c r="F14">
-        <v>7860</v>
+        <v>277132</v>
       </c>
       <c r="G14">
-        <v>408162.2</v>
+        <v>5551</v>
       </c>
       <c r="H14">
-        <v>277132</v>
+        <v>5337</v>
       </c>
       <c r="I14">
-        <v>5551</v>
+        <v>4.1</v>
       </c>
       <c r="J14">
-        <v>5337</v>
+        <v>40.9</v>
       </c>
       <c r="K14">
-        <v>4.1</v>
+        <v>1071</v>
       </c>
       <c r="L14">
-        <v>40.9</v>
+        <v>393.8</v>
       </c>
       <c r="M14">
-        <v>1071</v>
+        <v>96.3</v>
       </c>
       <c r="N14">
-        <v>393.8</v>
+        <v>4.2</v>
       </c>
       <c r="O14">
-        <v>96.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
+        <v>0.5</v>
+      </c>
+      <c r="R14">
+        <v>46.5</v>
+      </c>
+      <c r="S14">
+        <v>859.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>6232</v>
+      </c>
+      <c r="E15">
+        <v>328727.8</v>
       </c>
       <c r="F15">
-        <v>6232</v>
+        <v>253154</v>
       </c>
       <c r="G15">
-        <v>328727.8</v>
+        <v>4988</v>
       </c>
       <c r="H15">
-        <v>253154</v>
+        <v>4799</v>
       </c>
       <c r="I15">
-        <v>4988</v>
+        <v>4.8</v>
       </c>
       <c r="J15">
-        <v>4799</v>
+        <v>47.8</v>
       </c>
       <c r="K15">
-        <v>4.8</v>
+        <v>1269</v>
       </c>
       <c r="L15">
-        <v>47.8</v>
+        <v>491.3</v>
       </c>
       <c r="M15">
-        <v>1269</v>
+        <v>102.8</v>
       </c>
       <c r="N15">
-        <v>491.3</v>
+        <v>4.4</v>
       </c>
       <c r="O15">
-        <v>102.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>2.9</v>
+      </c>
+      <c r="P15">
+        <v>0.6</v>
+      </c>
+      <c r="Q15">
+        <v>0.4</v>
+      </c>
+      <c r="R15">
+        <v>55.8</v>
+      </c>
+      <c r="S15">
+        <v>1230.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>5552</v>
+      </c>
+      <c r="E16">
+        <v>288937.8</v>
       </c>
       <c r="F16">
-        <v>5552</v>
+        <v>266782</v>
       </c>
       <c r="G16">
-        <v>288937.8</v>
+        <v>5296</v>
       </c>
       <c r="H16">
-        <v>266782</v>
+        <v>5126</v>
       </c>
       <c r="I16">
-        <v>5296</v>
+        <v>5.5</v>
       </c>
       <c r="J16">
-        <v>5126</v>
+        <v>55.4</v>
       </c>
       <c r="K16">
-        <v>5.5</v>
+        <v>1446</v>
       </c>
       <c r="L16">
-        <v>55.4</v>
+        <v>534.3</v>
       </c>
       <c r="M16">
-        <v>1446</v>
+        <v>96.5</v>
       </c>
       <c r="N16">
-        <v>534.3</v>
+        <v>4</v>
       </c>
       <c r="O16">
-        <v>96.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>2.6</v>
+      </c>
+      <c r="P16">
+        <v>0.5</v>
+      </c>
+      <c r="Q16">
+        <v>0.5</v>
+      </c>
+      <c r="R16">
+        <v>43.6</v>
+      </c>
+      <c r="S16">
+        <v>685.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>38090</v>
+      </c>
+      <c r="E17">
+        <v>2240816.8</v>
       </c>
       <c r="F17">
-        <v>38090</v>
+        <v>449785</v>
       </c>
       <c r="G17">
-        <v>2240816.8</v>
+        <v>7414</v>
       </c>
       <c r="H17">
-        <v>449785</v>
+        <v>7646</v>
       </c>
       <c r="I17">
-        <v>7414</v>
+        <v>8.4</v>
       </c>
       <c r="J17">
-        <v>7646</v>
+        <v>84.5</v>
       </c>
       <c r="K17">
-        <v>8.4</v>
+        <v>2202</v>
       </c>
       <c r="L17">
-        <v>84.5</v>
+        <v>708.5</v>
       </c>
       <c r="M17">
-        <v>2202</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="N17">
-        <v>708.5</v>
+        <v>3.5</v>
       </c>
       <c r="O17">
-        <v>83.90000000000001</v>
+        <v>2.7</v>
+      </c>
+      <c r="P17">
+        <v>0.3</v>
+      </c>
+      <c r="Q17">
+        <v>0.7</v>
+      </c>
+      <c r="R17">
+        <v>51.2</v>
+      </c>
+      <c r="S17">
+        <v>1276.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>